<commit_message>
fix weird term in agdafair template metadata
</commit_message>
<xml_diff>
--- a/templates/community/AgDaFAIR/AgDaFAIR_potato_field_imaging_template_v0.1.0.xlsx
+++ b/templates/community/AgDaFAIR/AgDaFAIR_potato_field_imaging_template_v0.1.0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EFB347-629D-4729-A48B-959CB8886829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C115DDB-4A7C-4E7E-AEC1-26599EC7F6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,18 +90,12 @@
     <t>https://bioregistry.io/NCIT:C183327</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/ENVO2021_00000114</t>
-  </si>
-  <si>
     <t>Tags Term Source REF</t>
   </si>
   <si>
     <t>NCIT</t>
   </si>
   <si>
-    <t>envo</t>
-  </si>
-  <si>
     <t>Comment[description]</t>
   </si>
   <si>
@@ -337,16 +331,30 @@
   </si>
   <si>
     <t>AgDaFAIR</t>
+  </si>
+  <si>
+    <t>https://bioregistry.io/ENVO:00000114</t>
+  </si>
+  <si>
+    <t>ENVO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -369,13 +377,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -776,11 +787,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="136.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="114" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -824,7 +841,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -884,133 +901,136 @@
       <c r="C14" t="s">
         <v>23</v>
       </c>
-      <c r="D14" t="s">
-        <v>24</v>
+      <c r="D14" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D14" r:id="rId1" tooltip="https://bioregistry.io/envo:00000114" xr:uid="{17560985-F14B-4E34-A9AA-3170E84CBC04}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
@@ -1028,234 +1048,234 @@
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>58</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>59</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>60</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>63</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>64</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>65</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>66</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>68</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>69</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>70</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>71</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>72</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>73</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>74</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>75</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>76</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>77</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>78</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>79</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>83</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>85</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>86</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>87</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
         <v>90</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" t="s">
         <v>91</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>92</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M2" t="s">
+        <v>96</v>
+      </c>
+      <c r="N2" t="s">
+        <v>94</v>
+      </c>
+      <c r="O2" t="s">
+        <v>95</v>
+      </c>
+      <c r="P2" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>97</v>
+      </c>
+      <c r="R2" t="s">
+        <v>90</v>
+      </c>
+      <c r="S2" t="s">
+        <v>90</v>
+      </c>
+      <c r="T2" t="s">
+        <v>90</v>
+      </c>
+      <c r="U2" t="s">
+        <v>91</v>
+      </c>
+      <c r="V2" t="s">
         <v>92</v>
       </c>
-      <c r="E2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="W2" t="s">
         <v>93</v>
       </c>
-      <c r="H2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" t="s">
-        <v>97</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="X2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y2" t="s">
         <v>98</v>
       </c>
-      <c r="N2" t="s">
-        <v>96</v>
-      </c>
-      <c r="O2" t="s">
-        <v>97</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="Z2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC2" t="s">
         <v>98</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="AD2" t="s">
         <v>99</v>
       </c>
-      <c r="R2" t="s">
-        <v>92</v>
-      </c>
-      <c r="S2" t="s">
-        <v>92</v>
-      </c>
-      <c r="T2" t="s">
-        <v>92</v>
-      </c>
-      <c r="U2" t="s">
-        <v>93</v>
-      </c>
-      <c r="V2" t="s">
-        <v>94</v>
-      </c>
-      <c r="W2" t="s">
-        <v>95</v>
-      </c>
-      <c r="X2" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="AE2" t="s">
         <v>100</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AF2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG2" t="s">
         <v>101</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AH2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI2" t="s">
         <v>102</v>
       </c>
-      <c r="AB2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="AJ2" t="s">
         <v>103</v>
       </c>
-      <c r="AH2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>105</v>
-      </c>
       <c r="AK2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AL2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>